<commit_message>
initailized a mjml project
</commit_message>
<xml_diff>
--- a/src/data/Customers.xlsx
+++ b/src/data/Customers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\G PROJECT\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\G-Project\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDF9676-36C9-4E32-8660-4B1FB4554124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7390A32E-5D8C-4061-97DC-7AD6A0F06FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9CE7F7D-1182-4143-AA88-C3D9D0F7E835}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="122">
   <si>
     <t>Region</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -320,12 +320,180 @@
     <t>+1 403-273-4821</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>http://www.bobsbarricades.com/</t>
+  </si>
+  <si>
+    <t>jalter@bobsbarricades.com</t>
+  </si>
+  <si>
+    <t>+1 (407)-855-7186</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>French Barricades, Crowd Control Barrier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JOE ALTER (Senior Vice President:)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bob's Barricades, Inc.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>United States - FLORIDA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>921 Shotgun Road
+Sunrise, Florida 33326-1910</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crowd Control Warehouse</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>United States</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.crowdcontrolwarehouse.com/</t>
+  </si>
+  <si>
+    <t>sales@crowdcontrolwarehouse.com</t>
+  </si>
+  <si>
+    <t>+1 (877) 885-1600</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crowd Control Barrier</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crowd Control Direct, Inc.</t>
+  </si>
+  <si>
+    <t>https://www.crowdcontroldirect.com/</t>
+  </si>
+  <si>
+    <t>Crowd Control DIRECT, Inc.
+329 W 18th St. Suite 705
+Chicago, IL 60616</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sales@crowdcontroldirect.com</t>
+  </si>
+  <si>
+    <t>United Stated - Chicago</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crowd Control Solutions Ltd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2A Blackthorn House, St Paul's Square
+Birmingham, B3 1RL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.crowdcontrolsolutions.co.uk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uk - Birmingham</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0121 308 6441</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>+ 1 (773) 313-3900</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hello@crowdcontrolsolutions.co.uk</t>
+  </si>
+  <si>
+    <t>303 Butterworth Street New Orleans, LA 70121</t>
+  </si>
+  <si>
+    <t>+1 800-394-9294</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Friedrichs Custom Mfg., Inc.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sales@barricades.net</t>
+  </si>
+  <si>
+    <t>https://www.barricades.net/</t>
+  </si>
+  <si>
+    <t>United Stated - New Orleans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>oliveccanada@gmail.com</t>
+  </si>
+  <si>
+    <t>https://globalfence.ca/</t>
+  </si>
+  <si>
+    <t>Olivec Canada</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Canada</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>k9kennelsstore@gmail.com</t>
+  </si>
+  <si>
+    <t>+1 888-642-8889</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>+1 801-621-4024</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>833 West 27th Street, Ogden, Ut 84401</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All kinds of Fence</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customized Fence (For dogs)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://k9-kennelstore.com/</t>
+  </si>
+  <si>
+    <t>K9 KENNEL STORE COMPANY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +542,22 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -400,7 +584,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -422,10 +606,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -444,6 +637,436 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>397809</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>175000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3104029</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>505760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2" descr="Bob's logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FCBB6E2-7E69-4226-AD42-9AAE312C9937}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5249956" y="7705353"/>
+          <a:ext cx="2706220" cy="330760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2839010</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>511548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3" descr="Crowd Control Warehouse">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85FF8763-7026-0CE8-AF79-E912A412CAB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5300382" y="8202705"/>
+          <a:ext cx="2390775" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>745192</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2526102</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4" descr="crowd control direct">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{362D9812-E94B-CDE4-14C5-38B3FFAE8B21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5597339" y="8785412"/>
+          <a:ext cx="1780910" cy="627529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>521074</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2510117</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>498372</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5" descr="Crowd Control Solutions">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{989EF3B2-2F0D-043D-BB62-8F096FAB4C73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5373221" y="9547411"/>
+          <a:ext cx="1989043" cy="363902"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>851647</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2400830</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>593911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="图片 6" descr="Barricade picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7740425D-E7EA-E81E-E081-CFAC7AAEFE92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5703794" y="10118912"/>
+          <a:ext cx="1549183" cy="515470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1277471</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2017059</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>557911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="图片 7" descr="Olivec Canada">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF582FB-D6E2-F1FD-CF03-F554180B09B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6420971" y="10735235"/>
+          <a:ext cx="739588" cy="490676"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>616323</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2622176</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>582137</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8" descr="K9 Kennels">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76EED977-3C06-DBF9-0373-47E0D3C2CCC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5759823" y="11329146"/>
+          <a:ext cx="2005853" cy="548520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -743,30 +1366,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5EAC22F-6D7C-4B4D-8FAB-757F833940FE}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.75" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="47.75" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="109.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.25" style="2" customWidth="1"/>
     <col min="7" max="7" width="29.25" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.25" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.25" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.875" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,7 +1427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -820,21 +1443,18 @@
       <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="10" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8">
-        <f ca="1">NOW()-(16/24)</f>
-        <v>44776.901037152784</v>
-      </c>
+      <c r="I2" s="7"/>
       <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -854,7 +1474,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -864,6 +1484,9 @@
       <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
@@ -871,7 +1494,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -881,6 +1504,9 @@
       <c r="D5" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="G5" s="5" t="s">
         <v>33</v>
       </c>
@@ -888,7 +1514,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -911,7 +1537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
@@ -931,7 +1557,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
@@ -951,7 +1577,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
@@ -971,7 +1597,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
@@ -984,14 +1610,14 @@
       <c r="E10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="10" t="s">
         <v>65</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
@@ -1004,14 +1630,14 @@
       <c r="E11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="10" t="s">
         <v>66</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
@@ -1029,6 +1655,176 @@
       </c>
       <c r="H12" s="5" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1040,16 +1836,24 @@
     <hyperlink ref="D5" r:id="rId4" xr:uid="{86204D2F-A027-47AB-9E35-02B53FC52841}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{88C874FB-EF32-41ED-933A-08CB5D5C199D}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{7290C8BA-D769-44EA-AC6E-1C86B8763F02}"/>
-    <hyperlink ref="G2" r:id="rId7" xr:uid="{8246C970-6CA1-481B-AF05-848A9FE2990B}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{15C26473-D3FF-481B-9CC5-3972C8AEB5EE}"/>
-    <hyperlink ref="D9" r:id="rId9" xr:uid="{C5269D9F-5C79-4F4B-BA39-5B410C9740EA}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{C56DD2A7-F041-4784-9FC9-E847F20B8D69}"/>
-    <hyperlink ref="G10" r:id="rId11" xr:uid="{19AD085F-9E33-4A2D-B863-9B8DE98F1637}"/>
-    <hyperlink ref="G11" r:id="rId12" xr:uid="{743A592B-E511-4309-92B9-8EB73362986B}"/>
-    <hyperlink ref="D11" r:id="rId13" xr:uid="{B48ED5F4-B255-4280-9C70-A21270DC4E05}"/>
-    <hyperlink ref="D12" r:id="rId14" xr:uid="{F5AFE33F-91CA-4605-86D4-B37D4D538A32}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{15C26473-D3FF-481B-9CC5-3972C8AEB5EE}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{C5269D9F-5C79-4F4B-BA39-5B410C9740EA}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{C56DD2A7-F041-4784-9FC9-E847F20B8D69}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{B48ED5F4-B255-4280-9C70-A21270DC4E05}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{F5AFE33F-91CA-4605-86D4-B37D4D538A32}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{E0858346-22D9-4786-8CBB-0B1CA3954602}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{C8363C00-4B0E-4C4E-809B-EF681198F6C8}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{A8DD1C1D-967D-42F3-8D05-F9E0DE04A970}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{041FD575-4EE3-4AF8-BD2A-EE490A92F196}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{42A660DD-2BDE-4C51-B543-407A760DBE2C}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{13D0B075-7F65-40D2-98E4-8BDF8B86C3E2}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{6AA97D4C-5314-44FE-8FDC-07E110734A31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <ignoredErrors>
+    <ignoredError sqref="H4" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create a new email template
</commit_message>
<xml_diff>
--- a/src/data/Customers.xlsx
+++ b/src/data/Customers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\G-Project\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7390A32E-5D8C-4061-97DC-7AD6A0F06FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7653CD8F-05D1-48C9-B2C2-E5D486041E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9CE7F7D-1182-4143-AA88-C3D9D0F7E835}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="138">
   <si>
     <t>Region</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -487,6 +487,63 @@
   </si>
   <si>
     <t>K9 KENNEL STORE COMPANY</t>
+  </si>
+  <si>
+    <t>https://challengerfence.com/</t>
+  </si>
+  <si>
+    <t>Challenger Fence Inc.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>53 Kentucky Ave, Paterson NJ, 07503</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>+1 973-772-2593</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buckley Fence, LLC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sales@challengerfence.com</t>
+  </si>
+  <si>
+    <t>6000 E. 49th Ave. Drive Unit 10 Commerce City, Colorado 80022</t>
+  </si>
+  <si>
+    <t>Sales@BuckleyFence.com</t>
+  </si>
+  <si>
+    <t>+1 866-604-4076</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.buckleyfence.com/</t>
+  </si>
+  <si>
+    <t>Iron Fence and chain link fence</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wambam Fence</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://wambamfence.com/</t>
+  </si>
+  <si>
+    <t>hmmm@wambamfence.com</t>
+  </si>
+  <si>
+    <t>6935 Unit K Reames Rd, Charlotte NC, 28216</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>+1 877-778-5733</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -584,7 +641,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -614,9 +671,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -764,15 +818,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>745192</xdr:colOff>
+      <xdr:colOff>902075</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2526102</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>2364442</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>560110</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -802,8 +856,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5597339" y="8785412"/>
-          <a:ext cx="1780910" cy="627529"/>
+          <a:off x="6045575" y="8830236"/>
+          <a:ext cx="1462367" cy="515286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1048,6 +1102,189 @@
         <a:xfrm>
           <a:off x="5759823" y="11329146"/>
           <a:ext cx="2005853" cy="548520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1008530</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2073089</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>583480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1" descr="Challenger Fence Inc. Logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DB64675-73EC-8F0E-CFCE-71BD541E4F96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6152030" y="12001500"/>
+          <a:ext cx="1064559" cy="505039"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>885265</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>568818</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="图片 9" descr="Horse Fencing">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A76B32A-7190-A588-65F0-7F2C9FB48836}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6028765" y="12617824"/>
+          <a:ext cx="1210235" cy="501582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>963706</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2196353</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>627301</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="图片 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ACA7B86-B756-B4F5-C03D-4B2FD514E7C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6107206" y="13245353"/>
+          <a:ext cx="1232647" cy="560066"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1366,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5EAC22F-6D7C-4B4D-8FAB-757F833940FE}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1443,7 +1680,7 @@
       <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -1610,7 +1847,7 @@
       <c r="E10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -1630,7 +1867,7 @@
       <c r="E11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -1783,7 +2020,7 @@
       <c r="A18" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>111</v>
       </c>
       <c r="C18"/>
@@ -1825,6 +2062,75 @@
       </c>
       <c r="L19" s="2" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1848,12 +2154,15 @@
     <hyperlink ref="D17" r:id="rId16" xr:uid="{42A660DD-2BDE-4C51-B543-407A760DBE2C}"/>
     <hyperlink ref="D18" r:id="rId17" xr:uid="{13D0B075-7F65-40D2-98E4-8BDF8B86C3E2}"/>
     <hyperlink ref="D19" r:id="rId18" xr:uid="{6AA97D4C-5314-44FE-8FDC-07E110734A31}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{089B501E-CCB7-477F-AF3E-D181053ACCD0}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{E57379C7-279C-42B6-B18C-04BB05F8E71B}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{39FEE6A4-699F-4118-AE20-2A3CCACF5BD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
   <ignoredErrors>
     <ignoredError sqref="H4" numberStoredAsText="1"/>
   </ignoredErrors>
-  <drawing r:id="rId20"/>
+  <drawing r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>